<commit_message>
xong bug giai đoạn từng
</commit_message>
<xml_diff>
--- a/DongAERP/Content/Report/ReportHSDetailt/ReportHSDetailLTGradationForGaration.xlsx
+++ b/DongAERP/Content/Report/ReportHSDetailt/ReportHSDetailLTGradationForGaration.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DongAERP\DongAERP\Content\Report\ReportHSDetailt\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9B27C2-ACF7-4907-AC91-97C5938D3584}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2633C857-EECD-4AB5-8B9C-A6134543DEF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{FDADBC8A-6B6C-45FD-98E5-87326587A42E}"/>
   </bookViews>
@@ -33,18 +33,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
-  <si>
-    <t>Đơn vị:</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Tổng</t>
   </si>
   <si>
     <t>USD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Quy USD </t>
   </si>
   <si>
     <t>Thị trường</t>
@@ -65,7 +59,7 @@
     <t>GBP</t>
   </si>
   <si>
-    <t>BÁO CÁO CHI TIẾT - HỒ SƠ CHI TRẢ THEO THỊ TRƯỜNG - LOẠI HÌNH CHI TRẢ</t>
+    <t>BÁO CÁO CHI TIẾT - HỒ SƠ CHI TRẢ THEO THỊ TRƯỜNG - LOẠI TIỀN</t>
   </si>
 </sst>
 </file>
@@ -221,12 +215,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -244,6 +232,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -590,18 +584,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="21" x14ac:dyDescent="0.4">
-      <c r="B1" s="20" t="s">
-        <v>10</v>
+      <c r="B1" s="18" t="s">
+        <v>8</v>
       </c>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
@@ -614,17 +608,17 @@
       <c r="U1" s="4"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
       <c r="L2" s="5"/>
       <c r="M2" s="5"/>
       <c r="N2" s="5"/>
@@ -637,17 +631,17 @@
       <c r="U2" s="5"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A3" s="21"/>
-      <c r="B3" s="21"/>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
+      <c r="A3" s="19"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -1782,48 +1776,44 @@
       <c r="M74" s="6"/>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="N80" s="1" t="s">
+      <c r="N80" s="1"/>
+      <c r="O80" s="1"/>
+    </row>
+    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A81" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="B81" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C81" s="15"/>
+      <c r="D81" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E81" s="17"/>
+      <c r="F81" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="15"/>
+      <c r="H81" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="I81" s="17"/>
+      <c r="J81" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="K81" s="15"/>
+      <c r="L81" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="M81" s="17"/>
+      <c r="N81" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="O80" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B81" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="C81" s="17"/>
-      <c r="D81" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E81" s="19"/>
-      <c r="F81" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="G81" s="17"/>
-      <c r="H81" s="18" t="s">
-        <v>7</v>
-      </c>
-      <c r="I81" s="19"/>
-      <c r="J81" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="K81" s="17"/>
-      <c r="L81" s="18" t="s">
-        <v>9</v>
-      </c>
-      <c r="M81" s="19"/>
-      <c r="N81" s="16" t="s">
-        <v>1</v>
-      </c>
-      <c r="O81" s="17"/>
+      <c r="O81" s="15"/>
     </row>
     <row r="82" spans="1:15" ht="13.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A82" s="15"/>
+      <c r="A82" s="21"/>
       <c r="B82" s="13"/>
       <c r="C82" s="13"/>
       <c r="D82" s="13"/>

</xml_diff>